<commit_message>
Final figs for WQ4
</commit_message>
<xml_diff>
--- a/water_quality/data/samples.xlsx
+++ b/water_quality/data/samples.xlsx
@@ -2141,13 +2141,13 @@
         <v>7.93</v>
       </c>
       <c r="E38" s="7">
+        <v>33620.0</v>
+      </c>
+      <c r="F38" s="7">
         <v>48980.0</v>
       </c>
-      <c r="F38" s="7">
+      <c r="G38" s="7">
         <v>30890.0</v>
-      </c>
-      <c r="G38" s="7">
-        <v>33620.0</v>
       </c>
       <c r="H38" s="7">
         <v>0.19</v>
@@ -2197,13 +2197,13 @@
         <v>8.12</v>
       </c>
       <c r="E39" s="7">
+        <v>35390.0</v>
+      </c>
+      <c r="F39" s="7">
         <v>51830.0</v>
       </c>
-      <c r="F39" s="7">
+      <c r="G39" s="7">
         <v>32460.0</v>
-      </c>
-      <c r="G39" s="7">
-        <v>35390.0</v>
       </c>
       <c r="H39" s="7">
         <v>0.32</v>
@@ -2253,13 +2253,13 @@
         <v>8.21</v>
       </c>
       <c r="E40" s="7">
+        <v>35440.0</v>
+      </c>
+      <c r="F40" s="7">
         <v>51330.0</v>
       </c>
-      <c r="F40" s="7">
+      <c r="G40" s="7">
         <v>32520.0</v>
-      </c>
-      <c r="G40" s="7">
-        <v>35440.0</v>
       </c>
       <c r="H40" s="7">
         <v>0.36</v>
@@ -2309,13 +2309,13 @@
         <v>8.1</v>
       </c>
       <c r="E41" s="7">
+        <v>35590.0</v>
+      </c>
+      <c r="F41" s="7">
         <v>51410.0</v>
       </c>
-      <c r="F41" s="7">
+      <c r="G41" s="7">
         <v>32210.0</v>
-      </c>
-      <c r="G41" s="7">
-        <v>35590.0</v>
       </c>
       <c r="H41" s="7">
         <v>0.53</v>
@@ -2365,13 +2365,13 @@
         <v>8.11</v>
       </c>
       <c r="E42" s="7">
+        <v>35790.0</v>
+      </c>
+      <c r="F42" s="7">
         <v>51520.0</v>
       </c>
-      <c r="F42" s="7">
+      <c r="G42" s="7">
         <v>32630.0</v>
-      </c>
-      <c r="G42" s="7">
-        <v>35790.0</v>
       </c>
       <c r="H42" s="7">
         <v>0.37</v>
@@ -2421,13 +2421,13 @@
         <v>7.98</v>
       </c>
       <c r="E43" s="7">
+        <v>35610.0</v>
+      </c>
+      <c r="F43" s="7">
         <v>51920.0</v>
       </c>
-      <c r="F43" s="7">
+      <c r="G43" s="7">
         <v>32650.0</v>
-      </c>
-      <c r="G43" s="7">
-        <v>35610.0</v>
       </c>
       <c r="H43" s="7">
         <v>1.2</v>
@@ -2477,13 +2477,13 @@
         <v>7.83</v>
       </c>
       <c r="E44" s="7">
+        <v>36260.0</v>
+      </c>
+      <c r="F44" s="7">
         <v>50570.0</v>
       </c>
-      <c r="F44" s="7">
+      <c r="G44" s="7">
         <v>32240.0</v>
-      </c>
-      <c r="G44" s="7">
-        <v>36260.0</v>
       </c>
       <c r="H44" s="7">
         <v>2.22</v>
@@ -2533,13 +2533,13 @@
         <v>7.89</v>
       </c>
       <c r="E45" s="7">
+        <v>34980.0</v>
+      </c>
+      <c r="F45" s="7">
         <v>50620.0</v>
       </c>
-      <c r="F45" s="7">
+      <c r="G45" s="7">
         <v>32070.0</v>
-      </c>
-      <c r="G45" s="7">
-        <v>34980.0</v>
       </c>
       <c r="H45" s="7">
         <v>0.93</v>
@@ -2589,13 +2589,13 @@
         <v>8.11</v>
       </c>
       <c r="E46" s="7">
+        <v>34590.0</v>
+      </c>
+      <c r="F46" s="7">
         <v>49990.0</v>
       </c>
-      <c r="F46" s="7">
+      <c r="G46" s="7">
         <v>31730.0</v>
-      </c>
-      <c r="G46" s="7">
-        <v>34590.0</v>
       </c>
       <c r="H46" s="7">
         <v>0.87</v>
@@ -2645,13 +2645,13 @@
         <v>8.01</v>
       </c>
       <c r="E47" s="7">
+        <v>34770.0</v>
+      </c>
+      <c r="F47" s="7">
         <v>50440.0</v>
       </c>
-      <c r="F47" s="7">
+      <c r="G47" s="7">
         <v>31940.0</v>
-      </c>
-      <c r="G47" s="7">
-        <v>34770.0</v>
       </c>
       <c r="H47" s="7">
         <v>0.56</v>
@@ -2701,13 +2701,13 @@
         <v>7.79</v>
       </c>
       <c r="E48" s="7">
+        <v>35270.0</v>
+      </c>
+      <c r="F48" s="7">
         <v>51090.0</v>
       </c>
-      <c r="F48" s="7">
+      <c r="G48" s="7">
         <v>32450.0</v>
-      </c>
-      <c r="G48" s="7">
-        <v>35270.0</v>
       </c>
       <c r="H48" s="7">
         <v>3.52</v>
@@ -2757,13 +2757,13 @@
         <v>7.86</v>
       </c>
       <c r="E49" s="7">
+        <v>34950.0</v>
+      </c>
+      <c r="F49" s="7">
         <v>50560.0</v>
       </c>
-      <c r="F49" s="7">
+      <c r="G49" s="7">
         <v>32090.0</v>
-      </c>
-      <c r="G49" s="7">
-        <v>34950.0</v>
       </c>
       <c r="H49" s="7">
         <v>0.96</v>
@@ -2813,13 +2813,13 @@
         <v>7.88</v>
       </c>
       <c r="E50" s="7">
+        <v>34480.0</v>
+      </c>
+      <c r="F50" s="7">
         <v>50010.0</v>
       </c>
-      <c r="F50" s="7">
+      <c r="G50" s="7">
         <v>31530.0</v>
-      </c>
-      <c r="G50" s="7">
-        <v>34480.0</v>
       </c>
       <c r="H50" s="7">
         <v>0.89</v>
@@ -2869,13 +2869,13 @@
         <v>8.22</v>
       </c>
       <c r="E51" s="7">
+        <v>33270.0</v>
+      </c>
+      <c r="F51" s="7">
         <v>47430.0</v>
       </c>
-      <c r="F51" s="7">
+      <c r="G51" s="7">
         <v>30320.0</v>
-      </c>
-      <c r="G51" s="7">
-        <v>33270.0</v>
       </c>
       <c r="H51" s="7">
         <v>0.43</v>
@@ -2925,13 +2925,13 @@
         <v>8.15</v>
       </c>
       <c r="E52" s="7">
+        <v>33500.0</v>
+      </c>
+      <c r="F52" s="7">
         <v>48830.0</v>
       </c>
-      <c r="F52" s="7">
+      <c r="G52" s="7">
         <v>30830.0</v>
-      </c>
-      <c r="G52" s="7">
-        <v>33500.0</v>
       </c>
       <c r="H52" s="7">
         <v>0.45</v>
@@ -2981,13 +2981,13 @@
         <v>8.23</v>
       </c>
       <c r="E53" s="7">
+        <v>34960.0</v>
+      </c>
+      <c r="F53" s="7">
         <v>50660.0</v>
       </c>
-      <c r="F53" s="7">
+      <c r="G53" s="7">
         <v>30600.0</v>
-      </c>
-      <c r="G53" s="7">
-        <v>34960.0</v>
       </c>
       <c r="H53" s="7">
         <v>0.86</v>

</xml_diff>